<commit_message>
data added, header and navbar added, more scrapers added, changed and added images to database, added basic map images, added few icons and placeholder banner
</commit_message>
<xml_diff>
--- a/docs/dfdsfs.xlsx
+++ b/docs/dfdsfs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -24,13 +24,10 @@
     <t xml:space="preserve">need 1-4</t>
   </si>
   <si>
-    <t xml:space="preserve">hard 0-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">now </t>
-  </si>
-  <si>
-    <t>abilities</t>
+    <t>battle</t>
+  </si>
+  <si>
+    <t>pokemon_game_location</t>
   </si>
   <si>
     <t>items</t>
@@ -54,15 +51,9 @@
     <t>moves</t>
   </si>
   <si>
-    <t>nature</t>
-  </si>
-  <si>
     <t>platforms</t>
   </si>
   <si>
-    <t>pokeball</t>
-  </si>
-  <si>
     <t>pokedex</t>
   </si>
   <si>
@@ -81,7 +72,7 @@
     <t>pokemon_learn_move</t>
   </si>
   <si>
-    <t>pokemon_game_location</t>
+    <t>trainer</t>
   </si>
   <si>
     <t>pokemon_national</t>
@@ -91,18 +82,6 @@
   </si>
   <si>
     <t>pokemon_type</t>
-  </si>
-  <si>
-    <t>character</t>
-  </si>
-  <si>
-    <t>pokemon_instance</t>
-  </si>
-  <si>
-    <t>teams</t>
-  </si>
-  <si>
-    <t>team_stage</t>
   </si>
   <si>
     <t>type</t>
@@ -143,7 +122,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -160,30 +140,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table1" ref="B2:F29">
-  <autoFilter ref="B2:F29">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="0"/>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters blank="1">
-        <filter val="3"/>
-        <filter val="4"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="F2:F29">
-    <sortCondition descending="0" ref="F2:F29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table1" ref="B2:D24">
+  <autoFilter ref="B2:D24"/>
+  <sortState ref="C2:C24">
+    <sortCondition descending="0" ref="C2:C24"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="3">
     <tableColumn id="1" name="name"/>
     <tableColumn id="2" name="ready 0-2"/>
     <tableColumn id="3" name="need 1-4"/>
-    <tableColumn id="4" name="hard 0-2"/>
-    <tableColumn id="5" name="now "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -691,7 +656,6 @@
     <col customWidth="1" min="2" max="2" width="25.421875"/>
     <col customWidth="1" min="3" max="3" width="12.140625"/>
     <col customWidth="1" min="4" max="4" width="12.57421875"/>
-    <col customWidth="1" min="5" max="5" width="12.140625"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.25">
@@ -704,233 +668,176 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" ht="14.25">
+      <c r="B3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" hidden="1">
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" hidden="1">
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" hidden="1">
+    </row>
+    <row r="5" ht="14.25">
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" hidden="1">
-      <c r="B6" t="s">
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" hidden="1">
-      <c r="B7" t="s">
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25" hidden="1">
-      <c r="B8" t="s">
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25" hidden="1">
-      <c r="B9" t="s">
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25" hidden="1">
-      <c r="B10" t="s">
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" hidden="1">
-      <c r="B11" t="s">
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" hidden="1">
-      <c r="B12" t="s">
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25" hidden="1">
-      <c r="B13" t="s">
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25" hidden="1">
-      <c r="B14" t="s">
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25" hidden="1">
-      <c r="B15" t="s">
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" hidden="1">
-      <c r="B16" t="s">
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" hidden="1">
-      <c r="B17" t="s">
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" hidden="1">
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>4</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
       <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" ht="14.25">
       <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25" hidden="1">
-      <c r="B21" t="s">
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" t="s">
         <v>23</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" hidden="1">
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25" hidden="1">
-      <c r="B23" t="s">
-        <v>25</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -938,88 +845,15 @@
     </row>
     <row r="24" ht="14.25">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>4</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25">
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25" hidden="1">
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25" hidden="1">
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-    </row>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25"/>
+    <row r="26" ht="14.25"/>
+    <row r="27" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>